<commit_message>
Apply first round of advisor's review
</commit_message>
<xml_diff>
--- a/dissertation/images/carmo_rosetta_times/carmo_rosetta_times.xlsx
+++ b/dissertation/images/carmo_rosetta_times/carmo_rosetta_times.xlsx
@@ -155,11 +155,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="114132480"/>
-        <c:axId val="114134016"/>
+        <c:axId val="113849856"/>
+        <c:axId val="113851392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114132480"/>
+        <c:axId val="113849856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -168,7 +168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114134016"/>
+        <c:crossAx val="113851392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -176,7 +176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114134016"/>
+        <c:axId val="113851392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -206,7 +206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114132480"/>
+        <c:crossAx val="113849856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -221,6 +221,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -241,7 +246,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="299" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="20" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -253,7 +258,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="7979276" cy="3417303"/>
+    <xdr:ext cx="7995903" cy="3434097"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>

</xml_diff>